<commit_message>
Actualizacion reporte de errores
</commit_message>
<xml_diff>
--- a/PREGAME/1.ELICITACION/1.7REPORTE_DE_ERRORES/G6_ReporteDeErrores_v1.0.xlsx
+++ b/PREGAME/1.ELICITACION/1.7REPORTE_DE_ERRORES/G6_ReporteDeErrores_v1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santy\Documents\ESPE\6 Oct-Feb\AseguramientoCalidadSoftware\U2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santy\Documents\ESPE\6 Oct-Feb\AseguramientoCalidadSoftware\GIT_ACSW\15360_G6_ACSW\PREGAME\1.ELICITACION\1.7REPORTE_DE_ERRORES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8C4FB4-A8DD-4FA6-BE53-47F8CD57FE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE360E0-069E-432A-88F8-FBC579B6E7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,6 +398,68 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -408,68 +470,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -487,6 +487,304 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>554181</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>24530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>5777345</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>5095103</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F50353CB-C2A4-40E0-9B13-552E5318578B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="789708" y="5109148"/>
+          <a:ext cx="10668001" cy="5070573"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7875948D-80AB-4337-8D4F-56CAA384F502}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="228600" y="10264140"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6EB5722-9986-4CDE-9B5F-9DB0E54002DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="228600" y="11193780"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="AutoShape 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52CB9600-A589-4022-AE16-C2705CF6495B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16207740" y="5074920"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2022765</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>138545</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4046175</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101736</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1215D54A-DBE6-431F-AF5C-921F3F5195BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2258292" y="10543309"/>
+          <a:ext cx="7468247" cy="6904318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>207819</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>110836</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6277800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>50782</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AE8FC0F-D4C2-4C38-B148-596A2F1C6950}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="443346" y="17650691"/>
+          <a:ext cx="11514818" cy="2461473"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -775,17 +1073,17 @@
   </sheetPr>
   <dimension ref="B1:K38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="45.77734375" customWidth="1"/>
-    <col min="3" max="3" width="3.77734375" customWidth="1"/>
-    <col min="4" max="4" width="45.77734375" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" customWidth="1"/>
+    <col min="4" max="4" width="102.77734375" customWidth="1"/>
     <col min="5" max="5" width="3.77734375" customWidth="1"/>
     <col min="6" max="6" width="3.33203125" customWidth="1"/>
   </cols>
@@ -799,207 +1097,206 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="2:11" s="6" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="7"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="2:11" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="11"/>
-      <c r="D3" s="36">
+      <c r="D3" s="27">
         <v>45314</v>
       </c>
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="29" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:11" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="40"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" spans="2:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="2:11" ht="130.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="13"/>
-      <c r="K7" s="43"/>
+      <c r="K7" s="30"/>
     </row>
     <row r="8" spans="2:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="2:11" ht="250.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+    </row>
+    <row r="9" spans="2:11" ht="408.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="43"/>
     </row>
     <row r="10" spans="2:11" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="31"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
     </row>
     <row r="13" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="2:11" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="31"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="31"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="31"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="2:8" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="2:8" s="5" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="2:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="27"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="25" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:8" ht="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1029,5 +1326,6 @@
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="95" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>